<commit_message>
Added description of how to manage ActivityName rolback and added Tests
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/ActivityChange RollbackAnalysis.xlsx
+++ b/Documentation/Design Analysis/ActivityChange RollbackAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14569207-8031-4A02-A0C1-DBAA9F535FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD1B23-B120-4330-8DC2-8411F44199BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{FC44FF1F-09FD-4F19-B1DB-BA525A069443}"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FC44FF1F-09FD-4F19-B1DB-BA525A069443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="28">
   <si>
     <t>Entries</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>New Entry is Added</t>
+  </si>
+  <si>
+    <t>New entry without same Activity Added</t>
+  </si>
+  <si>
+    <t>No new Entry Added</t>
+  </si>
+  <si>
+    <t>New entry with same Activity Added</t>
+  </si>
+  <si>
+    <t>New entry with same Activity and one without Added</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -224,6 +236,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -232,11 +253,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -250,6 +268,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent6" xfId="4" builtinId="49"/>
@@ -674,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B2C700-84BA-44BC-860C-AA9E471A0047}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,21 +712,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="G1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -857,13 +881,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="G9">
         <v>7</v>
       </c>
@@ -932,7 +956,7 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="13" t="b">
+      <c r="E13" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -946,7 +970,7 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="13" t="b">
+      <c r="E14" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -968,52 +992,52 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="3" t="b">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="b">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1230,54 +1254,54 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>8</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="A28" s="2">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2">
         <v>12</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3" t="b">
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>9</v>
-      </c>
-      <c r="B29" s="3">
-        <v>13</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="3" t="b">
+      <c r="A29" s="2">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="G31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="G31" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1494,171 +1518,189 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>8</v>
-      </c>
-      <c r="B40" s="3">
+      <c r="A40" s="2">
+        <v>8</v>
+      </c>
+      <c r="B40" s="2">
         <v>12</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="3" t="b">
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3">
-        <v>13</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="13" t="b">
+      <c r="A41" s="2">
+        <v>9</v>
+      </c>
+      <c r="B41" s="2">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>10</v>
       </c>
-      <c r="B42" s="2">
-        <v>13</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="B42" s="1">
+        <v>13</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>3</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>12</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="6" t="b">
+      <c r="C46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>6</v>
-      </c>
-      <c r="B47" s="8">
+      <c r="A47" s="6">
+        <v>6</v>
+      </c>
+      <c r="B47" s="7">
         <v>12</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="9" t="b">
+      <c r="C47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
-        <v>8</v>
-      </c>
-      <c r="B48" s="11">
+      <c r="A48" s="9">
+        <v>9</v>
+      </c>
+      <c r="B48" s="10">
         <v>12</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="12" t="b">
+      <c r="C48" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>4</v>
-      </c>
-      <c r="B51" s="5">
-        <v>13</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="6" t="b">
+      <c r="A51" s="3">
+        <v>4</v>
+      </c>
+      <c r="B51" s="4">
+        <v>13</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
-        <v>7</v>
-      </c>
-      <c r="B52" s="8">
-        <v>13</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9" t="b">
+      <c r="A52" s="6">
+        <v>7</v>
+      </c>
+      <c r="B52" s="7">
+        <v>13</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
-        <v>9</v>
-      </c>
-      <c r="B53" s="8">
-        <v>13</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="14" t="b">
+      <c r="A53" s="6">
+        <v>9</v>
+      </c>
+      <c r="B53" s="7">
+        <v>13</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
-        <v>9</v>
-      </c>
-      <c r="B54" s="11">
-        <v>13</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="12" t="b">
+      <c r="A54" s="9">
+        <v>10</v>
+      </c>
+      <c r="B54" s="10">
+        <v>13</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="11" t="b">
         <v>0</v>
       </c>
       <c r="F54" t="s">
@@ -1666,61 +1708,163 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>3</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B57" s="4">
         <v>12</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
-        <v>6</v>
-      </c>
-      <c r="B57" s="8">
+      <c r="C57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>6</v>
+      </c>
+      <c r="B58" s="7">
         <v>12</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="10">
-        <v>9</v>
-      </c>
-      <c r="B58" s="11">
+      <c r="C58" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>8</v>
+      </c>
+      <c r="B59" s="7">
         <v>12</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>23</v>
+      <c r="C59" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>4</v>
+      </c>
+      <c r="B62" s="4">
+        <v>13</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>7</v>
+      </c>
+      <c r="B63" s="7">
+        <v>13</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>9</v>
+      </c>
+      <c r="B64" s="7">
+        <v>13</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>10</v>
+      </c>
+      <c r="B65" s="7">
+        <v>13</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>11</v>
+      </c>
+      <c r="B66" s="7">
+        <v>13</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A61:E61"/>
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>